<commit_message>
[FIX] add activity_group in line Asset and fix bug text, filter group
</commit_message>
<xml_diff>
--- a/pabi_budget_drilldown_report/xlsx_template/budget_invest_asset_report.xlsx
+++ b/pabi_budget_drilldown_report/xlsx_template/budget_invest_asset_report.xlsx
@@ -82,7 +82,7 @@
     <t xml:space="preserve">Actual</t>
   </si>
   <si>
-    <t xml:space="preserve">Toal Spent</t>
+    <t xml:space="preserve">Total Spent</t>
   </si>
   <si>
     <t xml:space="preserve">Balance</t>
@@ -304,8 +304,8 @@
   </sheetPr>
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -354,7 +354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" s="8" customFormat="true" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="8" customFormat="true" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
[FIX] budget report at invest_asset and invest_construction
</commit_message>
<xml_diff>
--- a/pabi_budget_drilldown_report/xlsx_template/budget_invest_asset_report.xlsx
+++ b/pabi_budget_drilldown_report/xlsx_template/budget_invest_asset_report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Budget Asset Report</t>
   </si>
@@ -43,22 +43,10 @@
     <t xml:space="preserve">Org</t>
   </si>
   <si>
-    <t xml:space="preserve">Division</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Section Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Section Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Investment Asset Code</t>
   </si>
   <si>
     <t xml:space="preserve">Investment Asset Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status</t>
   </si>
   <si>
     <t xml:space="preserve">Budget Plan</t>
@@ -302,23 +290,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="35.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="7" style="2" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="2" width="15.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="35.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="2" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="2" width="15.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="16" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,18 +388,10 @@
       <c r="O9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="AMG9" s="0"/>
+      <c r="AMH9" s="0"/>
+      <c r="AMI9" s="0"/>
+      <c r="AMJ9" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[ADD] Column and show 'ดึงไม่ได้'
</commit_message>
<xml_diff>
--- a/pabi_budget_drilldown_report/xlsx_template/budget_invest_asset_report.xlsx
+++ b/pabi_budget_drilldown_report/xlsx_template/budget_invest_asset_report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Budget Asset Report</t>
   </si>
@@ -43,10 +43,22 @@
     <t xml:space="preserve">Org</t>
   </si>
   <si>
+    <t xml:space="preserve">Division</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Investment Asset Code</t>
   </si>
   <si>
     <t xml:space="preserve">Investment Asset Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
   </si>
   <si>
     <t xml:space="preserve">Budget Plan</t>
@@ -290,23 +302,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="35.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="2" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="2" width="15.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1020" min="16" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="35.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="7" style="2" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="2" width="15.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="2" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,10 +400,18 @@
       <c r="O9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AMG9" s="0"/>
-      <c r="AMH9" s="0"/>
-      <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
+      <c r="P9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[FIX] asset budget report
</commit_message>
<xml_diff>
--- a/pabi_budget_drilldown_report/xlsx_template/budget_invest_asset_report.xlsx
+++ b/pabi_budget_drilldown_report/xlsx_template/budget_invest_asset_report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Budget Asset Report</t>
   </si>
@@ -43,7 +43,10 @@
     <t xml:space="preserve">Org</t>
   </si>
   <si>
-    <t xml:space="preserve">Division</t>
+    <t xml:space="preserve">Division Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Division Name</t>
   </si>
   <si>
     <t xml:space="preserve">Section Code</t>
@@ -302,23 +305,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="35.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="7" style="2" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="2" width="15.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="16.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="35.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="8" style="2" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="2" width="15.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="2" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -411,6 +416,9 @@
       </c>
       <c r="S9" s="7" t="s">
         <v>24</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>